<commit_message>
S- and SPY- learners fix TeacherGridWorld updated Teacher provide the size of the observation tree
</commit_message>
<xml_diff>
--- a/data/results/Mealy_R5.xlsx
+++ b/data/results/Mealy_R5.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="40">
   <si>
     <t>Correct</t>
   </si>
@@ -652,10 +652,11 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % – Zvýraznění1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4248,19 +4249,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:AF26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="13" max="13" width="9.140625" style="2"/>
+    <col min="13" max="14" width="9.140625" style="2"/>
+    <col min="15" max="21" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -4297,8 +4299,59 @@
       <c r="M1" s="2">
         <v>0.56578899999999999</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="3">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="3">
+        <v>76</v>
+      </c>
+      <c r="R1" s="3">
+        <v>96</v>
+      </c>
+      <c r="S1" s="3">
+        <v>3.8</v>
+      </c>
+      <c r="T1" s="3">
+        <v>43</v>
+      </c>
+      <c r="U1" s="3">
+        <v>0.56578899999999999</v>
+      </c>
+      <c r="W1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X1">
+        <v>20</v>
+      </c>
+      <c r="Y1">
+        <v>76</v>
+      </c>
+      <c r="Z1" s="2">
+        <v>0.56578899999999999</v>
+      </c>
+      <c r="AA1">
+        <v>59</v>
+      </c>
+      <c r="AB1">
+        <v>280</v>
+      </c>
+      <c r="AC1" s="2">
+        <v>0.46071400000000001</v>
+      </c>
+      <c r="AD1">
+        <v>174</v>
+      </c>
+      <c r="AE1">
+        <v>1015</v>
+      </c>
+      <c r="AF1" s="2">
+        <v>0.37930999999999998</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -4335,8 +4388,59 @@
       <c r="M2" s="2">
         <v>0.54545500000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="3">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>88</v>
+      </c>
+      <c r="R2" s="3">
+        <v>111</v>
+      </c>
+      <c r="S2" s="3">
+        <v>3.8260869999999998</v>
+      </c>
+      <c r="T2" s="3">
+        <v>48</v>
+      </c>
+      <c r="U2" s="3">
+        <v>0.54545500000000002</v>
+      </c>
+      <c r="W2" t="s">
+        <v>33</v>
+      </c>
+      <c r="X2">
+        <v>23</v>
+      </c>
+      <c r="Y2">
+        <v>88</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>0.54545500000000002</v>
+      </c>
+      <c r="AA2">
+        <v>68</v>
+      </c>
+      <c r="AB2">
+        <v>330</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>0.43939400000000001</v>
+      </c>
+      <c r="AD2">
+        <v>203</v>
+      </c>
+      <c r="AE2">
+        <v>1192</v>
+      </c>
+      <c r="AF2" s="2">
+        <v>0.36577199999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -4373,8 +4477,59 @@
       <c r="M3" s="2">
         <v>0.58750000000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="3">
+        <v>20</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>80</v>
+      </c>
+      <c r="R3" s="3">
+        <v>100</v>
+      </c>
+      <c r="S3" s="3">
+        <v>4</v>
+      </c>
+      <c r="T3" s="3">
+        <v>47</v>
+      </c>
+      <c r="U3" s="3">
+        <v>0.58750000000000002</v>
+      </c>
+      <c r="W3" t="s">
+        <v>34</v>
+      </c>
+      <c r="X3">
+        <v>20</v>
+      </c>
+      <c r="Y3">
+        <v>80</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>0.58750000000000002</v>
+      </c>
+      <c r="AA3">
+        <v>59</v>
+      </c>
+      <c r="AB3">
+        <v>293</v>
+      </c>
+      <c r="AC3" s="2">
+        <v>0.48464200000000002</v>
+      </c>
+      <c r="AD3">
+        <v>174</v>
+      </c>
+      <c r="AE3">
+        <v>1055</v>
+      </c>
+      <c r="AF3" s="2">
+        <v>0.40284399999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -4411,8 +4566,59 @@
       <c r="M4" s="2">
         <v>0.59722200000000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P4" s="3">
+        <v>19</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>72</v>
+      </c>
+      <c r="R4" s="3">
+        <v>91</v>
+      </c>
+      <c r="S4" s="3">
+        <v>3.7894739999999998</v>
+      </c>
+      <c r="T4" s="3">
+        <v>43</v>
+      </c>
+      <c r="U4" s="3">
+        <v>0.59722200000000003</v>
+      </c>
+      <c r="W4" t="s">
+        <v>35</v>
+      </c>
+      <c r="X4">
+        <v>19</v>
+      </c>
+      <c r="Y4">
+        <v>72</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>0.59722200000000003</v>
+      </c>
+      <c r="AA4">
+        <v>56</v>
+      </c>
+      <c r="AB4">
+        <v>279</v>
+      </c>
+      <c r="AC4" s="2">
+        <v>0.47670299999999999</v>
+      </c>
+      <c r="AD4">
+        <v>168</v>
+      </c>
+      <c r="AE4">
+        <v>1003</v>
+      </c>
+      <c r="AF4" s="2">
+        <v>0.39581300000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -4449,8 +4655,59 @@
       <c r="M5" s="2">
         <v>0.82089599999999996</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P5" s="3">
+        <v>12</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>67</v>
+      </c>
+      <c r="R5" s="3">
+        <v>79</v>
+      </c>
+      <c r="S5" s="3">
+        <v>5.5833329999999997</v>
+      </c>
+      <c r="T5" s="3">
+        <v>55</v>
+      </c>
+      <c r="U5" s="3">
+        <v>0.82089599999999996</v>
+      </c>
+      <c r="W5" t="s">
+        <v>36</v>
+      </c>
+      <c r="X5">
+        <v>12</v>
+      </c>
+      <c r="Y5">
+        <v>67</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>0.82089599999999996</v>
+      </c>
+      <c r="AA5">
+        <v>39</v>
+      </c>
+      <c r="AB5">
+        <v>257</v>
+      </c>
+      <c r="AC5" s="2">
+        <v>0.67704299999999995</v>
+      </c>
+      <c r="AD5">
+        <v>124</v>
+      </c>
+      <c r="AE5">
+        <v>913</v>
+      </c>
+      <c r="AF5" s="2">
+        <v>0.56188400000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -4487,8 +4744,59 @@
       <c r="M6" s="2">
         <v>0.85483900000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P6" s="3">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>62</v>
+      </c>
+      <c r="R6" s="3">
+        <v>72</v>
+      </c>
+      <c r="S6" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="T6" s="3">
+        <v>53</v>
+      </c>
+      <c r="U6" s="3">
+        <v>0.85483900000000002</v>
+      </c>
+      <c r="W6" t="s">
+        <v>37</v>
+      </c>
+      <c r="X6">
+        <v>10</v>
+      </c>
+      <c r="Y6">
+        <v>62</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>0.85483900000000002</v>
+      </c>
+      <c r="AA6">
+        <v>37</v>
+      </c>
+      <c r="AB6">
+        <v>243</v>
+      </c>
+      <c r="AC6" s="2">
+        <v>0.68312799999999996</v>
+      </c>
+      <c r="AD6">
+        <v>108</v>
+      </c>
+      <c r="AE6">
+        <v>859</v>
+      </c>
+      <c r="AF6" s="2">
+        <v>0.610012</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -4525,8 +4833,59 @@
       <c r="M7" s="2">
         <v>0.614286</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P7" s="3">
+        <v>17</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>70</v>
+      </c>
+      <c r="R7" s="3">
+        <v>87</v>
+      </c>
+      <c r="S7" s="3">
+        <v>4.1176469999999998</v>
+      </c>
+      <c r="T7" s="3">
+        <v>43</v>
+      </c>
+      <c r="U7" s="3">
+        <v>0.614286</v>
+      </c>
+      <c r="W7" t="s">
+        <v>38</v>
+      </c>
+      <c r="X7">
+        <v>17</v>
+      </c>
+      <c r="Y7">
+        <v>70</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>0.614286</v>
+      </c>
+      <c r="AA7">
+        <v>44</v>
+      </c>
+      <c r="AB7">
+        <v>254</v>
+      </c>
+      <c r="AC7" s="2">
+        <v>0.52362200000000003</v>
+      </c>
+      <c r="AD7">
+        <v>130</v>
+      </c>
+      <c r="AE7">
+        <v>893</v>
+      </c>
+      <c r="AF7" s="2">
+        <v>0.44456899999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -4563,8 +4922,59 @@
       <c r="M8" s="2">
         <v>0.86363599999999996</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="P8" s="3">
+        <v>10</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>66</v>
+      </c>
+      <c r="R8" s="3">
+        <v>76</v>
+      </c>
+      <c r="S8" s="3">
+        <v>6.6</v>
+      </c>
+      <c r="T8" s="3">
+        <v>57</v>
+      </c>
+      <c r="U8" s="3">
+        <v>0.86363599999999996</v>
+      </c>
+      <c r="W8" t="s">
+        <v>39</v>
+      </c>
+      <c r="X8">
+        <v>10</v>
+      </c>
+      <c r="Y8">
+        <v>66</v>
+      </c>
+      <c r="Z8" s="2">
+        <v>0.86363599999999996</v>
+      </c>
+      <c r="AA8">
+        <v>28</v>
+      </c>
+      <c r="AB8">
+        <v>231</v>
+      </c>
+      <c r="AC8" s="2">
+        <v>0.770563</v>
+      </c>
+      <c r="AD8">
+        <v>84</v>
+      </c>
+      <c r="AE8">
+        <v>807</v>
+      </c>
+      <c r="AF8" s="2">
+        <v>0.68153699999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -4601,8 +5011,29 @@
       <c r="M10" s="2">
         <v>0.46071400000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P10" s="3">
+        <v>59</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>280</v>
+      </c>
+      <c r="R10" s="3">
+        <v>339</v>
+      </c>
+      <c r="S10" s="3">
+        <v>4.7457630000000002</v>
+      </c>
+      <c r="T10" s="3">
+        <v>129</v>
+      </c>
+      <c r="U10" s="3">
+        <v>0.46071400000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -4639,8 +5070,29 @@
       <c r="M11" s="2">
         <v>0.43939400000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P11" s="3">
+        <v>68</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>330</v>
+      </c>
+      <c r="R11" s="3">
+        <v>398</v>
+      </c>
+      <c r="S11" s="3">
+        <v>4.8529410000000004</v>
+      </c>
+      <c r="T11" s="3">
+        <v>145</v>
+      </c>
+      <c r="U11" s="3">
+        <v>0.43939400000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -4677,8 +5129,29 @@
       <c r="M12" s="2">
         <v>0.48464200000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="P12" s="3">
+        <v>59</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>293</v>
+      </c>
+      <c r="R12" s="3">
+        <v>352</v>
+      </c>
+      <c r="S12" s="3">
+        <v>4.9661020000000002</v>
+      </c>
+      <c r="T12" s="3">
+        <v>142</v>
+      </c>
+      <c r="U12" s="3">
+        <v>0.48464200000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -4715,8 +5188,29 @@
       <c r="M13" s="2">
         <v>0.47670299999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P13" s="3">
+        <v>56</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>279</v>
+      </c>
+      <c r="R13" s="3">
+        <v>335</v>
+      </c>
+      <c r="S13" s="3">
+        <v>4.9821429999999998</v>
+      </c>
+      <c r="T13" s="3">
+        <v>133</v>
+      </c>
+      <c r="U13" s="3">
+        <v>0.47670299999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -4753,8 +5247,29 @@
       <c r="M14" s="2">
         <v>0.67704299999999995</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P14" s="3">
+        <v>39</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>257</v>
+      </c>
+      <c r="R14" s="3">
+        <v>296</v>
+      </c>
+      <c r="S14" s="3">
+        <v>6.5897439999999996</v>
+      </c>
+      <c r="T14" s="3">
+        <v>174</v>
+      </c>
+      <c r="U14" s="3">
+        <v>0.67704299999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -4791,8 +5306,29 @@
       <c r="M15" s="2">
         <v>0.68312799999999996</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P15" s="3">
+        <v>37</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>243</v>
+      </c>
+      <c r="R15" s="3">
+        <v>280</v>
+      </c>
+      <c r="S15" s="3">
+        <v>6.5675679999999996</v>
+      </c>
+      <c r="T15" s="3">
+        <v>166</v>
+      </c>
+      <c r="U15" s="3">
+        <v>0.68312799999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -4829,8 +5365,29 @@
       <c r="M16" s="2">
         <v>0.52362200000000003</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P16" s="3">
+        <v>45</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>257</v>
+      </c>
+      <c r="R16" s="3">
+        <v>302</v>
+      </c>
+      <c r="S16" s="3">
+        <v>5.7111109999999998</v>
+      </c>
+      <c r="T16" s="3">
+        <v>133</v>
+      </c>
+      <c r="U16" s="3">
+        <v>0.51751000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -4867,8 +5424,29 @@
       <c r="M17" s="2">
         <v>0.770563</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="P17" s="3">
+        <v>29</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>234</v>
+      </c>
+      <c r="R17" s="3">
+        <v>263</v>
+      </c>
+      <c r="S17" s="3">
+        <v>8.0689659999999996</v>
+      </c>
+      <c r="T17" s="3">
+        <v>179</v>
+      </c>
+      <c r="U17" s="3">
+        <v>0.764957</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -4905,8 +5483,29 @@
       <c r="M19" s="2">
         <v>0.37930999999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P19" s="3">
+        <v>174</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>1015</v>
+      </c>
+      <c r="R19" s="3">
+        <v>1189</v>
+      </c>
+      <c r="S19" s="3">
+        <v>5.8333329999999997</v>
+      </c>
+      <c r="T19" s="3">
+        <v>385</v>
+      </c>
+      <c r="U19" s="3">
+        <v>0.37930999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -4943,8 +5542,29 @@
       <c r="M20" s="2">
         <v>0.36577199999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P20" s="3">
+        <v>203</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>1192</v>
+      </c>
+      <c r="R20" s="3">
+        <v>1395</v>
+      </c>
+      <c r="S20" s="3">
+        <v>5.8719210000000004</v>
+      </c>
+      <c r="T20" s="3">
+        <v>436</v>
+      </c>
+      <c r="U20" s="3">
+        <v>0.36577199999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -4981,8 +5601,29 @@
       <c r="M21" s="2">
         <v>0.40284399999999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O21" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="P21" s="3">
+        <v>174</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>1055</v>
+      </c>
+      <c r="R21" s="3">
+        <v>1229</v>
+      </c>
+      <c r="S21" s="3">
+        <v>6.063218</v>
+      </c>
+      <c r="T21" s="3">
+        <v>425</v>
+      </c>
+      <c r="U21" s="3">
+        <v>0.40284399999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -5019,8 +5660,29 @@
       <c r="M22" s="2">
         <v>0.39581300000000003</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O22" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P22" s="3">
+        <v>168</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>1003</v>
+      </c>
+      <c r="R22" s="3">
+        <v>1171</v>
+      </c>
+      <c r="S22" s="3">
+        <v>5.9702380000000002</v>
+      </c>
+      <c r="T22" s="3">
+        <v>397</v>
+      </c>
+      <c r="U22" s="3">
+        <v>0.39581300000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -5057,8 +5719,29 @@
       <c r="M23" s="2">
         <v>0.56188400000000005</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P23" s="3">
+        <v>124</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>913</v>
+      </c>
+      <c r="R23" s="3">
+        <v>1037</v>
+      </c>
+      <c r="S23" s="3">
+        <v>7.3629030000000002</v>
+      </c>
+      <c r="T23" s="3">
+        <v>513</v>
+      </c>
+      <c r="U23" s="3">
+        <v>0.56188400000000005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -5095,8 +5778,29 @@
       <c r="M24" s="2">
         <v>0.610012</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P24" s="3">
+        <v>108</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>859</v>
+      </c>
+      <c r="R24" s="3">
+        <v>967</v>
+      </c>
+      <c r="S24" s="3">
+        <v>7.9537040000000001</v>
+      </c>
+      <c r="T24" s="3">
+        <v>524</v>
+      </c>
+      <c r="U24" s="3">
+        <v>0.610012</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -5133,8 +5837,29 @@
       <c r="M25" s="2">
         <v>0.44456899999999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P25" s="3">
+        <v>131</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>930</v>
+      </c>
+      <c r="R25" s="3">
+        <v>1061</v>
+      </c>
+      <c r="S25" s="3">
+        <v>7.0992369999999996</v>
+      </c>
+      <c r="T25" s="3">
+        <v>399</v>
+      </c>
+      <c r="U25" s="3">
+        <v>0.42903200000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -5170,6 +5895,27 @@
       </c>
       <c r="M26" s="2">
         <v>0.68153699999999995</v>
+      </c>
+      <c r="O26" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="P26" s="3">
+        <v>84</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>807</v>
+      </c>
+      <c r="R26" s="3">
+        <v>891</v>
+      </c>
+      <c r="S26" s="3">
+        <v>9.6071430000000007</v>
+      </c>
+      <c r="T26" s="3">
+        <v>546</v>
+      </c>
+      <c r="U26" s="3">
+        <v>0.67657999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>